<commit_message>
Add measurement skill instruments
</commit_message>
<xml_diff>
--- a/exp2/case03/report/motivation/attention/MeasurementModel.xlsx
+++ b/exp2/case03/report/motivation/attention/MeasurementModel.xlsx
@@ -4598,25 +4598,25 @@
         <v>31</v>
       </c>
       <c r="B33" t="n" s="273">
-        <v>0.9608256925620914</v>
+        <v>0.9671138891831781</v>
       </c>
       <c r="C33" t="n" s="274">
-        <v>-0.12185404610554162</v>
+        <v>-0.09099795014767882</v>
       </c>
       <c r="D33" t="n" s="275">
-        <v>0.9030146102221674</v>
+        <v>0.9274942198452398</v>
       </c>
       <c r="E33" t="n" s="276">
         <v>1.0</v>
       </c>
       <c r="F33" t="n" s="277">
-        <v>0.9693477320011352</v>
+        <v>0.9763295184474029</v>
       </c>
       <c r="G33" t="n" s="278">
-        <v>-0.1100069381484669</v>
+        <v>-0.07620044202141216</v>
       </c>
       <c r="H33" t="n" s="279">
-        <v>0.9124038724666564</v>
+        <v>0.9392596310313256</v>
       </c>
       <c r="I33" t="n" s="280">
         <v>1.0</v>
@@ -4627,25 +4627,25 @@
         <v>32</v>
       </c>
       <c r="B34" t="n" s="273">
-        <v>0.7656779979459888</v>
+        <v>0.7664355098464104</v>
       </c>
       <c r="C34" t="n" s="274">
-        <v>-1.0428779393927068</v>
+        <v>-1.0359792543138695</v>
       </c>
       <c r="D34" t="n" s="275">
-        <v>0.2970048280756173</v>
+        <v>0.3002118210435647</v>
       </c>
       <c r="E34" t="n" s="276">
         <v>1.0</v>
       </c>
       <c r="F34" t="n" s="277">
-        <v>0.8022294905720919</v>
+        <v>0.7976913903735041</v>
       </c>
       <c r="G34" t="n" s="278">
-        <v>-0.9997041578870451</v>
+        <v>-1.0264797970038195</v>
       </c>
       <c r="H34" t="n" s="279">
-        <v>0.31745369930164</v>
+        <v>0.30466548175720154</v>
       </c>
       <c r="I34" t="n" s="280">
         <v>1.0</v>
@@ -4656,25 +4656,25 @@
         <v>33</v>
       </c>
       <c r="B35" t="n" s="273">
-        <v>0.7817177894337033</v>
+        <v>0.7900992218974096</v>
       </c>
       <c r="C35" t="n" s="274">
-        <v>-0.993089777757642</v>
+        <v>-0.9525732732209503</v>
       </c>
       <c r="D35" t="n" s="275">
-        <v>0.32066620512152455</v>
+        <v>0.34080632421888035</v>
       </c>
       <c r="E35" t="n" s="276">
         <v>1.0</v>
       </c>
       <c r="F35" t="n" s="277">
-        <v>0.8138639847842523</v>
+        <v>0.8256847857522598</v>
       </c>
       <c r="G35" t="n" s="278">
-        <v>-0.9402681733996655</v>
+        <v>-0.875695202731917</v>
       </c>
       <c r="H35" t="n" s="279">
-        <v>0.347080020457516</v>
+        <v>0.38119575400622935</v>
       </c>
       <c r="I35" t="n" s="280">
         <v>1.0</v>
@@ -4685,28 +4685,28 @@
         <v>34</v>
       </c>
       <c r="B36" t="n" s="273">
-        <v>1.3799443684514148</v>
+        <v>1.3625822262509124</v>
       </c>
       <c r="C36" t="n" s="274">
-        <v>1.5678367261750228</v>
+        <v>1.5165288097214866</v>
       </c>
       <c r="D36" t="n" s="275">
-        <v>0.11691924145805575</v>
+        <v>0.12938569117661755</v>
       </c>
       <c r="E36" t="n" s="276">
-        <v>0.8184346902063903</v>
+        <v>0.9056998382363228</v>
       </c>
       <c r="F36" t="n" s="277">
-        <v>1.4381112272307823</v>
+        <v>1.4213845792577826</v>
       </c>
       <c r="G36" t="n" s="278">
-        <v>1.9585165796916746</v>
+        <v>1.9004365111576846</v>
       </c>
       <c r="H36" t="n" s="279">
-        <v>0.05016942750322696</v>
+        <v>0.057375859311595515</v>
       </c>
       <c r="I36" t="n" s="280">
-        <v>0.35118599252258875</v>
+        <v>0.4016310151811686</v>
       </c>
     </row>
     <row r="37">
@@ -4714,25 +4714,25 @@
         <v>35</v>
       </c>
       <c r="B37" t="n" s="273">
-        <v>0.9807262575188614</v>
+        <v>0.9795882496791084</v>
       </c>
       <c r="C37" t="n" s="274">
-        <v>-0.05301858053341958</v>
+        <v>-0.05180868291482261</v>
       </c>
       <c r="D37" t="n" s="275">
-        <v>0.9577171034088803</v>
+        <v>0.9586811368793526</v>
       </c>
       <c r="E37" t="n" s="276">
         <v>1.0</v>
       </c>
       <c r="F37" t="n" s="277">
-        <v>0.9452594295729349</v>
+        <v>0.9543596169498801</v>
       </c>
       <c r="G37" t="n" s="278">
-        <v>-0.23929389808764548</v>
+        <v>-0.1894397498731145</v>
       </c>
       <c r="H37" t="n" s="279">
-        <v>0.8108776966098221</v>
+        <v>0.8497481725646348</v>
       </c>
       <c r="I37" t="n" s="280">
         <v>1.0</v>
@@ -4743,28 +4743,28 @@
         <v>58</v>
       </c>
       <c r="B38" t="n" s="273">
-        <v>1.1640609949086198</v>
+        <v>1.062056239712155</v>
       </c>
       <c r="C38" t="n" s="274">
-        <v>13.935027865643763</v>
+        <v>14.014455372042939</v>
       </c>
       <c r="D38" t="n" s="275">
-        <v>3.8804891535877617E-44</v>
+        <v>1.2717010894402588E-44</v>
       </c>
       <c r="E38" t="n" s="276">
-        <v>3.4924402382289855E-43</v>
+        <v>1.1445309804962329E-43</v>
       </c>
       <c r="F38" t="n" s="277">
-        <v>1.664792640554558</v>
+        <v>1.6265345062141163</v>
       </c>
       <c r="G38" t="n" s="278">
-        <v>2.1975885675276836</v>
+        <v>2.0690466148191864</v>
       </c>
       <c r="H38" t="n" s="279">
-        <v>0.027978438661370047</v>
+        <v>0.038541712610052424</v>
       </c>
       <c r="I38" t="n" s="280">
-        <v>0.22382750929096037</v>
+        <v>0.3083337008804194</v>
       </c>
     </row>
     <row r="39">
@@ -4772,28 +4772,28 @@
         <v>59</v>
       </c>
       <c r="B39" t="n" s="273">
-        <v>1.4619899122585565</v>
+        <v>1.4139622843394968</v>
       </c>
       <c r="C39" t="n" s="274">
-        <v>0.856953784463349</v>
+        <v>0.8377658286290536</v>
       </c>
       <c r="D39" t="n" s="275">
-        <v>0.39147042651562863</v>
+        <v>0.40216223389284034</v>
       </c>
       <c r="E39" t="n" s="276">
         <v>1.0</v>
       </c>
       <c r="F39" t="n" s="277">
-        <v>1.5331310736702197</v>
+        <v>1.521970161390382</v>
       </c>
       <c r="G39" t="n" s="278">
-        <v>3.6982187034192777</v>
+        <v>3.631771497394388</v>
       </c>
       <c r="H39" t="n" s="279">
-        <v>2.1711778340202252E-4</v>
+        <v>2.814823115464273E-4</v>
       </c>
       <c r="I39" t="n" s="280">
-        <v>0.002171177834020225</v>
+        <v>0.002814823115464273</v>
       </c>
     </row>
     <row r="40">
@@ -4801,25 +4801,25 @@
         <v>60</v>
       </c>
       <c r="B40" t="n" s="273">
-        <v>1.1006359136088097</v>
+        <v>1.076087277215562</v>
       </c>
       <c r="C40" t="n" s="274">
-        <v>0.7304339383912493</v>
+        <v>0.7122152503164044</v>
       </c>
       <c r="D40" t="n" s="275">
-        <v>0.46512497968422317</v>
+        <v>0.4763314947621274</v>
       </c>
       <c r="E40" t="n" s="276">
         <v>1.0</v>
       </c>
       <c r="F40" t="n" s="277">
-        <v>1.124735150707271</v>
+        <v>1.1159556704661209</v>
       </c>
       <c r="G40" t="n" s="278">
-        <v>0.9804077320060562</v>
+        <v>0.9646806039582434</v>
       </c>
       <c r="H40" t="n" s="279">
-        <v>0.32688489460852005</v>
+        <v>0.33470481310609534</v>
       </c>
       <c r="I40" t="n" s="280">
         <v>1.0</v>
@@ -4830,28 +4830,28 @@
         <v>61</v>
       </c>
       <c r="B41" t="n" s="273">
-        <v>1.1786498142723154</v>
+        <v>1.1668571653012678</v>
       </c>
       <c r="C41" t="n" s="274">
-        <v>4.185440731182603</v>
+        <v>3.9494754658988165</v>
       </c>
       <c r="D41" t="n" s="275">
-        <v>2.8461332708475266E-5</v>
+        <v>7.832263784256856E-5</v>
       </c>
       <c r="E41" t="n" s="276">
-        <v>2.2769066166780213E-4</v>
+        <v>6.265811027405485E-4</v>
       </c>
       <c r="F41" t="n" s="277">
-        <v>1.2842051516039663</v>
+        <v>1.2595825177034</v>
       </c>
       <c r="G41" t="n" s="278">
-        <v>2.5733168681608722</v>
+        <v>2.3664387524331634</v>
       </c>
       <c r="H41" t="n" s="279">
-        <v>0.010072893879377483</v>
+        <v>0.01796014569513867</v>
       </c>
       <c r="I41" t="n" s="280">
-        <v>0.09065604491439735</v>
+        <v>0.16164131125624803</v>
       </c>
     </row>
     <row r="42">
@@ -4859,10 +4859,10 @@
         <v>62</v>
       </c>
       <c r="B42" t="n" s="273">
-        <v>0.9739643353625448</v>
+        <v>1.026139269896127</v>
       </c>
       <c r="C42" t="n" s="274">
-        <v>122.08381970853654</v>
+        <v>109.65635931339207</v>
       </c>
       <c r="D42" t="n" s="275">
         <v>0.0</v>
@@ -4871,16 +4871,16 @@
         <v>0.0</v>
       </c>
       <c r="F42" t="n" s="277">
-        <v>1.4619439124155038</v>
+        <v>1.5381868251712103</v>
       </c>
       <c r="G42" t="n" s="278">
-        <v>5.310793313633997</v>
+        <v>5.978410901492728</v>
       </c>
       <c r="H42" t="n" s="279">
-        <v>1.0914906148324712E-7</v>
+        <v>2.253247958492748E-9</v>
       </c>
       <c r="I42" t="n" s="280">
-        <v>1.2006396763157183E-6</v>
+        <v>2.478572754342023E-8</v>
       </c>
     </row>
     <row r="43">
@@ -4888,10 +4888,10 @@
         <v>63</v>
       </c>
       <c r="B43" t="n" s="273">
-        <v>0.8980482166408296</v>
+        <v>0.9389805196729271</v>
       </c>
       <c r="C43" t="n" s="274">
-        <v>5779.157902120136</v>
+        <v>4902.4462785625765</v>
       </c>
       <c r="D43" t="n" s="275">
         <v>0.0</v>
@@ -4900,13 +4900,13 @@
         <v>0.0</v>
       </c>
       <c r="F43" t="n" s="277">
-        <v>1.1240202422173824</v>
+        <v>1.1711665427166746</v>
       </c>
       <c r="G43" t="n" s="278">
-        <v>0.9471646240793121</v>
+        <v>1.2791059200248978</v>
       </c>
       <c r="H43" t="n" s="279">
-        <v>0.34355489863610106</v>
+        <v>0.20085975919580862</v>
       </c>
       <c r="I43" t="n" s="280">
         <v>1.0</v>

</xml_diff>